<commit_message>
added a little information to Excel + added pictures of fichiers
</commit_message>
<xml_diff>
--- a/Fichiers analyse/FOSSE 1-4.xlsx
+++ b/Fichiers analyse/FOSSE 1-4.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cleme\Documents\GitHub\savoirs\cours\M2-pédologie\M2_EFT_projet_pedologie\Fichiers analyse\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a648334db5f9744c/M2_EFT_projet_pedologie/Fichiers analyse/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1523FAB1-26F5-4D24-B03C-72B0E9F713AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="80" documentId="13_ncr:1_{1523FAB1-26F5-4D24-B03C-72B0E9F713AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5986954-CBBC-4BE1-93D8-375E1E063016}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fosse1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1295" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1651" uniqueCount="93">
   <si>
     <t>Face</t>
   </si>
@@ -257,12 +257,75 @@
   <si>
     <t>https://appgeodb.nancy.inra.fr/biljou/fr/fiche/reserve-en-eau-du-sol</t>
   </si>
+  <si>
+    <t>0-10 cm</t>
+  </si>
+  <si>
+    <t>10-20 cm</t>
+  </si>
+  <si>
+    <t>20-30 cm</t>
+  </si>
+  <si>
+    <t>30-40 cm</t>
+  </si>
+  <si>
+    <t>40-50 cm</t>
+  </si>
+  <si>
+    <t>50-60 cm</t>
+  </si>
+  <si>
+    <t>60-70 cm</t>
+  </si>
+  <si>
+    <t>70-80 cm</t>
+  </si>
+  <si>
+    <t>80-90 cm</t>
+  </si>
+  <si>
+    <t>90-100 cm</t>
+  </si>
+  <si>
+    <t>Humidité</t>
+  </si>
+  <si>
+    <t>sec</t>
+  </si>
+  <si>
+    <t>frais</t>
+  </si>
+  <si>
+    <t>grumleux</t>
+  </si>
+  <si>
+    <t>sub-polyédrique</t>
+  </si>
+  <si>
+    <t>Structure_type</t>
+  </si>
+  <si>
+    <t>Structure_taille</t>
+  </si>
+  <si>
+    <t>lamellaire grossier</t>
+  </si>
+  <si>
+    <t>Compacité</t>
+  </si>
+  <si>
+    <t>compact</t>
+  </si>
+  <si>
+    <t>Taches</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -305,6 +368,27 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -326,7 +410,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -352,6 +436,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -573,10 +660,10 @@
   <dimension ref="A1:J1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:J1"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="6" width="12.6640625" customWidth="1"/>
   </cols>
@@ -4823,20 +4910,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J1000"/>
+  <dimension ref="A1:O1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:J1"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="O52" sqref="O52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.6640625" customWidth="1"/>
     <col min="2" max="2" width="11.44140625" customWidth="1"/>
     <col min="3" max="6" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>22</v>
       </c>
@@ -4867,8 +4954,23 @@
       <c r="J1" s="13" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K1" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="L1" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="M1" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="N1" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="O1" s="15" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -4900,8 +5002,20 @@
         <f>VLOOKUP($G2,Explications!$E$1:$G$16,3,0)*10*(1-$I2)/10</f>
         <v>1.35</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K2" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="L2" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="N2" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="O2" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -4933,8 +5047,20 @@
         <f>VLOOKUP($G3,Explications!$E$1:$G$16,3,0)*10*(1-$I3)/10</f>
         <v>1.35</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K3" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="L3" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="N3" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="O3" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -4966,8 +5092,20 @@
         <f>VLOOKUP($G4,Explications!$E$1:$G$16,3,0)*10*(1-$I4)/10</f>
         <v>1.35</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K4" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="L4" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="N4" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="O4" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -4999,8 +5137,20 @@
         <f>VLOOKUP($G5,Explications!$E$1:$G$16,3,0)*10*(1-$I5)/10</f>
         <v>1.35</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K5" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="L5" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="N5" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="O5" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -5032,8 +5182,20 @@
         <f>VLOOKUP($G6,Explications!$E$1:$G$16,3,0)*10*(1-$I6)/10</f>
         <v>1.35</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K6" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="L6" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="N6" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="O6" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -5065,8 +5227,20 @@
         <f>VLOOKUP($G7,Explications!$E$1:$G$16,3,0)*10*(1-$I7)/10</f>
         <v>1.35</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K7" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="L7" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="N7" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="O7" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -5098,8 +5272,20 @@
         <f>VLOOKUP($G8,Explications!$E$1:$G$16,3,0)*10*(1-$I8)/10</f>
         <v>1.35</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K8" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="L8" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="N8" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="O8" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -5131,8 +5317,20 @@
         <f>VLOOKUP($G9,Explications!$E$1:$G$16,3,0)*10*(1-$I9)/10</f>
         <v>1.35</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K9" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="L9" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="N9" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="O9" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -5164,8 +5362,20 @@
         <f>VLOOKUP($G10,Explications!$E$1:$G$16,3,0)*10*(1-$I10)/10</f>
         <v>1.35</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K10" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="L10" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="N10" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="O10" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -5197,8 +5407,20 @@
         <f>VLOOKUP($G11,Explications!$E$1:$G$16,3,0)*10*(1-$I11)/10</f>
         <v>1.35</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K11" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="L11" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="N11" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="O11" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -5230,8 +5452,20 @@
         <f>VLOOKUP($G12,Explications!$E$1:$G$16,3,0)*10*(1-$I12)/10</f>
         <v>1.2150000000000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K12" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L12" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="N12" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="O12" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -5263,8 +5497,20 @@
         <f>VLOOKUP($G13,Explications!$E$1:$G$16,3,0)*10*(1-$I13)/10</f>
         <v>1.2150000000000001</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K13" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L13" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="N13" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="O13" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -5296,8 +5542,20 @@
         <f>VLOOKUP($G14,Explications!$E$1:$G$16,3,0)*10*(1-$I14)/10</f>
         <v>1.2150000000000001</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K14" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L14" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="N14" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="O14" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
@@ -5329,8 +5587,20 @@
         <f>VLOOKUP($G15,Explications!$E$1:$G$16,3,0)*10*(1-$I15)/10</f>
         <v>1.2150000000000001</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K15" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L15" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="N15" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="O15" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
@@ -5362,8 +5632,20 @@
         <f>VLOOKUP($G16,Explications!$E$1:$G$16,3,0)*10*(1-$I16)/10</f>
         <v>1.2150000000000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K16" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L16" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="N16" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="O16" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>11</v>
       </c>
@@ -5395,8 +5677,20 @@
         <f>VLOOKUP($G17,Explications!$E$1:$G$16,3,0)*10*(1-$I17)/10</f>
         <v>1.2150000000000001</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K17" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L17" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="N17" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="O17" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>11</v>
       </c>
@@ -5428,8 +5722,20 @@
         <f>VLOOKUP($G18,Explications!$E$1:$G$16,3,0)*10*(1-$I18)/10</f>
         <v>1.2150000000000001</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K18" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L18" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="N18" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="O18" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>11</v>
       </c>
@@ -5461,8 +5767,20 @@
         <f>VLOOKUP($G19,Explications!$E$1:$G$16,3,0)*10*(1-$I19)/10</f>
         <v>1.2150000000000001</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K19" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L19" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="N19" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="O19" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>11</v>
       </c>
@@ -5494,8 +5812,20 @@
         <f>VLOOKUP($G20,Explications!$E$1:$G$16,3,0)*10*(1-$I20)/10</f>
         <v>1.2150000000000001</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K20" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L20" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="N20" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="O20" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>11</v>
       </c>
@@ -5527,8 +5857,20 @@
         <f>VLOOKUP($G21,Explications!$E$1:$G$16,3,0)*10*(1-$I21)/10</f>
         <v>1.2150000000000001</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K21" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L21" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="N21" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="O21" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>13</v>
       </c>
@@ -5560,8 +5902,20 @@
         <f>VLOOKUP($G22,Explications!$E$1:$G$16,3,0)*10*(1-$I22)/10</f>
         <v>1.2150000000000001</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K22" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L22" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="N22" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="O22" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>13</v>
       </c>
@@ -5593,8 +5947,20 @@
         <f>VLOOKUP($G23,Explications!$E$1:$G$16,3,0)*10*(1-$I23)/10</f>
         <v>1.2150000000000001</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K23" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L23" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="N23" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="O23" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>13</v>
       </c>
@@ -5626,8 +5992,20 @@
         <f>VLOOKUP($G24,Explications!$E$1:$G$16,3,0)*10*(1-$I24)/10</f>
         <v>1.2150000000000001</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K24" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L24" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="N24" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="O24" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>13</v>
       </c>
@@ -5659,8 +6037,20 @@
         <f>VLOOKUP($G25,Explications!$E$1:$G$16,3,0)*10*(1-$I25)/10</f>
         <v>1.2150000000000001</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K25" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L25" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="N25" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="O25" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>13</v>
       </c>
@@ -5692,8 +6082,20 @@
         <f>VLOOKUP($G26,Explications!$E$1:$G$16,3,0)*10*(1-$I26)/10</f>
         <v>1.2150000000000001</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K26" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L26" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="N26" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="O26" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>13</v>
       </c>
@@ -5725,8 +6127,20 @@
         <f>VLOOKUP($G27,Explications!$E$1:$G$16,3,0)*10*(1-$I27)/10</f>
         <v>1.2150000000000001</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K27" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L27" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="N27" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="O27" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>13</v>
       </c>
@@ -5758,8 +6172,20 @@
         <f>VLOOKUP($G28,Explications!$E$1:$G$16,3,0)*10*(1-$I28)/10</f>
         <v>1.2150000000000001</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K28" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L28" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="N28" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="O28" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>13</v>
       </c>
@@ -5791,8 +6217,20 @@
         <f>VLOOKUP($G29,Explications!$E$1:$G$16,3,0)*10*(1-$I29)/10</f>
         <v>1.2150000000000001</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K29" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L29" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="N29" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="O29" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>13</v>
       </c>
@@ -5824,8 +6262,20 @@
         <f>VLOOKUP($G30,Explications!$E$1:$G$16,3,0)*10*(1-$I30)/10</f>
         <v>1.2150000000000001</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K30" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L30" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="N30" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="O30" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>13</v>
       </c>
@@ -5857,8 +6307,20 @@
         <f>VLOOKUP($G31,Explications!$E$1:$G$16,3,0)*10*(1-$I31)/10</f>
         <v>1.2150000000000001</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K31" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L31" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="N31" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="O31" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>14</v>
       </c>
@@ -5890,8 +6352,20 @@
         <f>VLOOKUP($G32,Explications!$E$1:$G$16,3,0)*10*(1-$I32)/10</f>
         <v>1.0125</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K32" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L32" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="N32" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="O32" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>14</v>
       </c>
@@ -5923,8 +6397,20 @@
         <f>VLOOKUP($G33,Explications!$E$1:$G$16,3,0)*10*(1-$I33)/10</f>
         <v>1.0125</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K33" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L33" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="N33" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="O33" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>14</v>
       </c>
@@ -5956,8 +6442,20 @@
         <f>VLOOKUP($G34,Explications!$E$1:$G$16,3,0)*10*(1-$I34)/10</f>
         <v>1.0125</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K34" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L34" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="N34" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="O34" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>14</v>
       </c>
@@ -5989,8 +6487,20 @@
         <f>VLOOKUP($G35,Explications!$E$1:$G$16,3,0)*10*(1-$I35)/10</f>
         <v>1.0125</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K35" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L35" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="N35" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="O35" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>14</v>
       </c>
@@ -6022,8 +6532,20 @@
         <f>VLOOKUP($G36,Explications!$E$1:$G$16,3,0)*10*(1-$I36)/10</f>
         <v>1.0125</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K36" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L36" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="N36" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="O36" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>14</v>
       </c>
@@ -6055,8 +6577,20 @@
         <f>VLOOKUP($G37,Explications!$E$1:$G$16,3,0)*10*(1-$I37)/10</f>
         <v>1.0125</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K37" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L37" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="N37" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="O37" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>14</v>
       </c>
@@ -6088,8 +6622,20 @@
         <f>VLOOKUP($G38,Explications!$E$1:$G$16,3,0)*10*(1-$I38)/10</f>
         <v>1.0125</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K38" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L38" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="N38" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="O38" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>14</v>
       </c>
@@ -6121,8 +6667,20 @@
         <f>VLOOKUP($G39,Explications!$E$1:$G$16,3,0)*10*(1-$I39)/10</f>
         <v>1.0125</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K39" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L39" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="N39" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="O39" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>14</v>
       </c>
@@ -6154,8 +6712,20 @@
         <f>VLOOKUP($G40,Explications!$E$1:$G$16,3,0)*10*(1-$I40)/10</f>
         <v>1.0125</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K40" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L40" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="N40" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="O40" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>14</v>
       </c>
@@ -6187,8 +6757,20 @@
         <f>VLOOKUP($G41,Explications!$E$1:$G$16,3,0)*10*(1-$I41)/10</f>
         <v>1.0125</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K41" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L41" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="N41" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="O41" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>15</v>
       </c>
@@ -6220,8 +6802,20 @@
         <f>VLOOKUP($G42,Explications!$E$1:$G$16,3,0)*10*(1-$I42)/10</f>
         <v>0.74250000000000005</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K42" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L42" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N42" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="O42" s="17">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>15</v>
       </c>
@@ -6253,8 +6847,20 @@
         <f>VLOOKUP($G43,Explications!$E$1:$G$16,3,0)*10*(1-$I43)/10</f>
         <v>0.74250000000000005</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K43" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L43" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N43" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="O43" s="17">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>15</v>
       </c>
@@ -6286,8 +6892,20 @@
         <f>VLOOKUP($G44,Explications!$E$1:$G$16,3,0)*10*(1-$I44)/10</f>
         <v>0.74250000000000005</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K44" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L44" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N44" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="O44" s="17">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>15</v>
       </c>
@@ -6319,8 +6937,20 @@
         <f>VLOOKUP($G45,Explications!$E$1:$G$16,3,0)*10*(1-$I45)/10</f>
         <v>0.74250000000000005</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K45" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L45" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N45" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="O45" s="17">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>15</v>
       </c>
@@ -6352,8 +6982,20 @@
         <f>VLOOKUP($G46,Explications!$E$1:$G$16,3,0)*10*(1-$I46)/10</f>
         <v>0.74250000000000005</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K46" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L46" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N46" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="O46" s="17">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>15</v>
       </c>
@@ -6385,8 +7027,20 @@
         <f>VLOOKUP($G47,Explications!$E$1:$G$16,3,0)*10*(1-$I47)/10</f>
         <v>0.74250000000000005</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K47" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L47" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N47" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="O47" s="17">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>15</v>
       </c>
@@ -6418,8 +7072,20 @@
         <f>VLOOKUP($G48,Explications!$E$1:$G$16,3,0)*10*(1-$I48)/10</f>
         <v>0.74250000000000005</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K48" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L48" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N48" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="O48" s="17">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>15</v>
       </c>
@@ -6451,8 +7117,20 @@
         <f>VLOOKUP($G49,Explications!$E$1:$G$16,3,0)*10*(1-$I49)/10</f>
         <v>0.74250000000000005</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K49" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L49" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N49" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="O49" s="17">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>15</v>
       </c>
@@ -6484,8 +7162,20 @@
         <f>VLOOKUP($G50,Explications!$E$1:$G$16,3,0)*10*(1-$I50)/10</f>
         <v>0.74250000000000005</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K50" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L50" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N50" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="O50" s="17">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>15</v>
       </c>
@@ -6517,8 +7207,20 @@
         <f>VLOOKUP($G51,Explications!$E$1:$G$16,3,0)*10*(1-$I51)/10</f>
         <v>0.74250000000000005</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K51" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L51" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N51" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="O51" s="17">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>16</v>
       </c>
@@ -6550,8 +7252,17 @@
         <f>VLOOKUP($G52,Explications!$E$1:$G$16,3,0)*10*(1-$I52)/10</f>
         <v>0.74250000000000005</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K52" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L52" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N52" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>16</v>
       </c>
@@ -6583,8 +7294,17 @@
         <f>VLOOKUP($G53,Explications!$E$1:$G$16,3,0)*10*(1-$I53)/10</f>
         <v>0.74250000000000005</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K53" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L53" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N53" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>16</v>
       </c>
@@ -6616,8 +7336,17 @@
         <f>VLOOKUP($G54,Explications!$E$1:$G$16,3,0)*10*(1-$I54)/10</f>
         <v>0.74250000000000005</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K54" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L54" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N54" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>16</v>
       </c>
@@ -6649,8 +7378,17 @@
         <f>VLOOKUP($G55,Explications!$E$1:$G$16,3,0)*10*(1-$I55)/10</f>
         <v>0.74250000000000005</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K55" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L55" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N55" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>16</v>
       </c>
@@ -6682,8 +7420,17 @@
         <f>VLOOKUP($G56,Explications!$E$1:$G$16,3,0)*10*(1-$I56)/10</f>
         <v>0.74250000000000005</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K56" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L56" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N56" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>16</v>
       </c>
@@ -6715,8 +7462,17 @@
         <f>VLOOKUP($G57,Explications!$E$1:$G$16,3,0)*10*(1-$I57)/10</f>
         <v>0.74250000000000005</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K57" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L57" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N57" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>16</v>
       </c>
@@ -6748,8 +7504,17 @@
         <f>VLOOKUP($G58,Explications!$E$1:$G$16,3,0)*10*(1-$I58)/10</f>
         <v>0.74250000000000005</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K58" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L58" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N58" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>16</v>
       </c>
@@ -6781,8 +7546,17 @@
         <f>VLOOKUP($G59,Explications!$E$1:$G$16,3,0)*10*(1-$I59)/10</f>
         <v>0.74250000000000005</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K59" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L59" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N59" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>16</v>
       </c>
@@ -6814,8 +7588,17 @@
         <f>VLOOKUP($G60,Explications!$E$1:$G$16,3,0)*10*(1-$I60)/10</f>
         <v>0.74250000000000005</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K60" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L60" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N60" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>16</v>
       </c>
@@ -6847,8 +7630,17 @@
         <f>VLOOKUP($G61,Explications!$E$1:$G$16,3,0)*10*(1-$I61)/10</f>
         <v>0.74250000000000005</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K61" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L61" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N61" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>17</v>
       </c>
@@ -6880,8 +7672,17 @@
         <f>VLOOKUP($G62,Explications!$E$1:$G$16,3,0)*10*(1-$I62)/10</f>
         <v>0.74250000000000005</v>
       </c>
-    </row>
-    <row r="63" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K62" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L62" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N62" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>17</v>
       </c>
@@ -6913,8 +7714,17 @@
         <f>VLOOKUP($G63,Explications!$E$1:$G$16,3,0)*10*(1-$I63)/10</f>
         <v>0.74250000000000005</v>
       </c>
-    </row>
-    <row r="64" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K63" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L63" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N63" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>17</v>
       </c>
@@ -6946,8 +7756,17 @@
         <f>VLOOKUP($G64,Explications!$E$1:$G$16,3,0)*10*(1-$I64)/10</f>
         <v>0.74250000000000005</v>
       </c>
-    </row>
-    <row r="65" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K64" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L64" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N64" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>17</v>
       </c>
@@ -6979,8 +7798,17 @@
         <f>VLOOKUP($G65,Explications!$E$1:$G$16,3,0)*10*(1-$I65)/10</f>
         <v>0.74250000000000005</v>
       </c>
-    </row>
-    <row r="66" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K65" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L65" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N65" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>17</v>
       </c>
@@ -7012,8 +7840,17 @@
         <f>VLOOKUP($G66,Explications!$E$1:$G$16,3,0)*10*(1-$I66)/10</f>
         <v>0.74250000000000005</v>
       </c>
-    </row>
-    <row r="67" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K66" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L66" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N66" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>17</v>
       </c>
@@ -7045,8 +7882,17 @@
         <f>VLOOKUP($G67,Explications!$E$1:$G$16,3,0)*10*(1-$I67)/10</f>
         <v>0.74250000000000005</v>
       </c>
-    </row>
-    <row r="68" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K67" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L67" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N67" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>17</v>
       </c>
@@ -7078,8 +7924,17 @@
         <f>VLOOKUP($G68,Explications!$E$1:$G$16,3,0)*10*(1-$I68)/10</f>
         <v>0.74250000000000005</v>
       </c>
-    </row>
-    <row r="69" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K68" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L68" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N68" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>17</v>
       </c>
@@ -7111,8 +7966,17 @@
         <f>VLOOKUP($G69,Explications!$E$1:$G$16,3,0)*10*(1-$I69)/10</f>
         <v>0.74250000000000005</v>
       </c>
-    </row>
-    <row r="70" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K69" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L69" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N69" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>17</v>
       </c>
@@ -7144,8 +8008,17 @@
         <f>VLOOKUP($G70,Explications!$E$1:$G$16,3,0)*10*(1-$I70)/10</f>
         <v>0.74250000000000005</v>
       </c>
-    </row>
-    <row r="71" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K70" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L70" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N70" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>17</v>
       </c>
@@ -7177,8 +8050,17 @@
         <f>VLOOKUP($G71,Explications!$E$1:$G$16,3,0)*10*(1-$I71)/10</f>
         <v>0.74250000000000005</v>
       </c>
-    </row>
-    <row r="72" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K71" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L71" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N71" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>19</v>
       </c>
@@ -7210,8 +8092,17 @@
         <f>VLOOKUP($G72,Explications!$E$1:$G$16,3,0)*10*(1-$I72)/10</f>
         <v>1.4849999999999999</v>
       </c>
-    </row>
-    <row r="73" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K72" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L72" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N72" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>19</v>
       </c>
@@ -7243,8 +8134,17 @@
         <f>VLOOKUP($G73,Explications!$E$1:$G$16,3,0)*10*(1-$I73)/10</f>
         <v>1.4849999999999999</v>
       </c>
-    </row>
-    <row r="74" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K73" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L73" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N73" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>19</v>
       </c>
@@ -7276,8 +8176,17 @@
         <f>VLOOKUP($G74,Explications!$E$1:$G$16,3,0)*10*(1-$I74)/10</f>
         <v>1.4849999999999999</v>
       </c>
-    </row>
-    <row r="75" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K74" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L74" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N74" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>19</v>
       </c>
@@ -7309,8 +8218,17 @@
         <f>VLOOKUP($G75,Explications!$E$1:$G$16,3,0)*10*(1-$I75)/10</f>
         <v>1.4849999999999999</v>
       </c>
-    </row>
-    <row r="76" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K75" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L75" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N75" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>19</v>
       </c>
@@ -7342,8 +8260,17 @@
         <f>VLOOKUP($G76,Explications!$E$1:$G$16,3,0)*10*(1-$I76)/10</f>
         <v>1.4849999999999999</v>
       </c>
-    </row>
-    <row r="77" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K76" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L76" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N76" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>19</v>
       </c>
@@ -7375,8 +8302,17 @@
         <f>VLOOKUP($G77,Explications!$E$1:$G$16,3,0)*10*(1-$I77)/10</f>
         <v>1.4849999999999999</v>
       </c>
-    </row>
-    <row r="78" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K77" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L77" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N77" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>19</v>
       </c>
@@ -7408,8 +8344,17 @@
         <f>VLOOKUP($G78,Explications!$E$1:$G$16,3,0)*10*(1-$I78)/10</f>
         <v>1.4849999999999999</v>
       </c>
-    </row>
-    <row r="79" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K78" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L78" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N78" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>19</v>
       </c>
@@ -7441,8 +8386,17 @@
         <f>VLOOKUP($G79,Explications!$E$1:$G$16,3,0)*10*(1-$I79)/10</f>
         <v>1.4849999999999999</v>
       </c>
-    </row>
-    <row r="80" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K79" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L79" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N79" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>19</v>
       </c>
@@ -7474,8 +8428,17 @@
         <f>VLOOKUP($G80,Explications!$E$1:$G$16,3,0)*10*(1-$I80)/10</f>
         <v>1.4849999999999999</v>
       </c>
-    </row>
-    <row r="81" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K80" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L80" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N80" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>19</v>
       </c>
@@ -7507,8 +8470,17 @@
         <f>VLOOKUP($G81,Explications!$E$1:$G$16,3,0)*10*(1-$I81)/10</f>
         <v>1.4849999999999999</v>
       </c>
-    </row>
-    <row r="82" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K81" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L81" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N81" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>20</v>
       </c>
@@ -7540,8 +8512,17 @@
         <f>VLOOKUP($G82,Explications!$E$1:$G$16,3,0)*10*(1-$I82)/10</f>
         <v>1.4849999999999999</v>
       </c>
-    </row>
-    <row r="83" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K82" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L82" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N82" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>20</v>
       </c>
@@ -7573,8 +8554,17 @@
         <f>VLOOKUP($G83,Explications!$E$1:$G$16,3,0)*10*(1-$I83)/10</f>
         <v>1.4849999999999999</v>
       </c>
-    </row>
-    <row r="84" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K83" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L83" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N83" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>20</v>
       </c>
@@ -7606,8 +8596,17 @@
         <f>VLOOKUP($G84,Explications!$E$1:$G$16,3,0)*10*(1-$I84)/10</f>
         <v>1.4849999999999999</v>
       </c>
-    </row>
-    <row r="85" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K84" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L84" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N84" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>20</v>
       </c>
@@ -7639,8 +8638,17 @@
         <f>VLOOKUP($G85,Explications!$E$1:$G$16,3,0)*10*(1-$I85)/10</f>
         <v>1.4849999999999999</v>
       </c>
-    </row>
-    <row r="86" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K85" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L85" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N85" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>20</v>
       </c>
@@ -7672,8 +8680,17 @@
         <f>VLOOKUP($G86,Explications!$E$1:$G$16,3,0)*10*(1-$I86)/10</f>
         <v>1.4849999999999999</v>
       </c>
-    </row>
-    <row r="87" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K86" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L86" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N86" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>20</v>
       </c>
@@ -7705,8 +8722,17 @@
         <f>VLOOKUP($G87,Explications!$E$1:$G$16,3,0)*10*(1-$I87)/10</f>
         <v>1.4849999999999999</v>
       </c>
-    </row>
-    <row r="88" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K87" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L87" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N87" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>20</v>
       </c>
@@ -7738,8 +8764,17 @@
         <f>VLOOKUP($G88,Explications!$E$1:$G$16,3,0)*10*(1-$I88)/10</f>
         <v>1.4849999999999999</v>
       </c>
-    </row>
-    <row r="89" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K88" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L88" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N88" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>20</v>
       </c>
@@ -7771,8 +8806,17 @@
         <f>VLOOKUP($G89,Explications!$E$1:$G$16,3,0)*10*(1-$I89)/10</f>
         <v>1.4849999999999999</v>
       </c>
-    </row>
-    <row r="90" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K89" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L89" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N89" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>20</v>
       </c>
@@ -7804,8 +8848,17 @@
         <f>VLOOKUP($G90,Explications!$E$1:$G$16,3,0)*10*(1-$I90)/10</f>
         <v>1.4849999999999999</v>
       </c>
-    </row>
-    <row r="91" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K90" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L90" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N90" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>20</v>
       </c>
@@ -7837,8 +8890,17 @@
         <f>VLOOKUP($G91,Explications!$E$1:$G$16,3,0)*10*(1-$I91)/10</f>
         <v>1.4849999999999999</v>
       </c>
-    </row>
-    <row r="92" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K91" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L91" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N91" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>21</v>
       </c>
@@ -7870,8 +8932,17 @@
         <f>VLOOKUP($G92,Explications!$E$1:$G$16,3,0)*10*(1-$I92)/10</f>
         <v>1.4849999999999999</v>
       </c>
-    </row>
-    <row r="93" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K92" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L92" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N92" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>21</v>
       </c>
@@ -7903,8 +8974,17 @@
         <f>VLOOKUP($G93,Explications!$E$1:$G$16,3,0)*10*(1-$I93)/10</f>
         <v>1.4849999999999999</v>
       </c>
-    </row>
-    <row r="94" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K93" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L93" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N93" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>21</v>
       </c>
@@ -7936,8 +9016,17 @@
         <f>VLOOKUP($G94,Explications!$E$1:$G$16,3,0)*10*(1-$I94)/10</f>
         <v>1.4849999999999999</v>
       </c>
-    </row>
-    <row r="95" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K94" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L94" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N94" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>21</v>
       </c>
@@ -7969,8 +9058,17 @@
         <f>VLOOKUP($G95,Explications!$E$1:$G$16,3,0)*10*(1-$I95)/10</f>
         <v>1.4849999999999999</v>
       </c>
-    </row>
-    <row r="96" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K95" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L95" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N95" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>21</v>
       </c>
@@ -8002,8 +9100,17 @@
         <f>VLOOKUP($G96,Explications!$E$1:$G$16,3,0)*10*(1-$I96)/10</f>
         <v>1.4849999999999999</v>
       </c>
-    </row>
-    <row r="97" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K96" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L96" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N96" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>21</v>
       </c>
@@ -8035,8 +9142,17 @@
         <f>VLOOKUP($G97,Explications!$E$1:$G$16,3,0)*10*(1-$I97)/10</f>
         <v>1.4849999999999999</v>
       </c>
-    </row>
-    <row r="98" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K97" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L97" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N97" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="98" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>21</v>
       </c>
@@ -8068,8 +9184,17 @@
         <f>VLOOKUP($G98,Explications!$E$1:$G$16,3,0)*10*(1-$I98)/10</f>
         <v>1.4849999999999999</v>
       </c>
-    </row>
-    <row r="99" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K98" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L98" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N98" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>21</v>
       </c>
@@ -8101,8 +9226,17 @@
         <f>VLOOKUP($G99,Explications!$E$1:$G$16,3,0)*10*(1-$I99)/10</f>
         <v>1.4849999999999999</v>
       </c>
-    </row>
-    <row r="100" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K99" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L99" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N99" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="100" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>21</v>
       </c>
@@ -8134,8 +9268,17 @@
         <f>VLOOKUP($G100,Explications!$E$1:$G$16,3,0)*10*(1-$I100)/10</f>
         <v>1.4849999999999999</v>
       </c>
-    </row>
-    <row r="101" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K100" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L100" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N100" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>21</v>
       </c>
@@ -8167,18 +9310,27 @@
         <f>VLOOKUP($G101,Explications!$E$1:$G$16,3,0)*10*(1-$I101)/10</f>
         <v>1.4849999999999999</v>
       </c>
-    </row>
-    <row r="102" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="103" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="104" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="105" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="106" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="107" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="108" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="109" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="110" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="111" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="112" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="K101" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L101" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N101" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="102" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="103" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="104" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="105" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="106" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="107" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="108" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="109" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="110" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="111" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="112" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="113" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="114" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="115" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9080,11 +10232,11 @@
   </sheetPr>
   <dimension ref="A1:AA1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:J1"/>
+    <sheetView topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="6" width="12.6640625" customWidth="1"/>
   </cols>
@@ -20650,11 +21802,11 @@
   </sheetPr>
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J1"/>
+    <sheetView topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="G72" sqref="G72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="6" width="12.6640625" customWidth="1"/>
   </cols>
@@ -24901,18 +26053,18 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:K1000"/>
+  <dimension ref="A1:M1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="6" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="3" t="s">
         <v>31</v>
@@ -24939,8 +26091,11 @@
       <c r="K1" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L1" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -24968,8 +26123,14 @@
       <c r="K2" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L2" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -24997,8 +26158,14 @@
       <c r="K3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L3" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" s="16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -25026,8 +26193,14 @@
       <c r="K4" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L4" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="M4" s="16" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -25055,8 +26228,14 @@
       <c r="K5" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L5" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="M5" s="16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D6" s="1" t="s">
         <v>52</v>
       </c>
@@ -25069,8 +26248,14 @@
       <c r="G6" s="10">
         <v>1.45</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L6" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="M6" s="16" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D7" s="1" t="s">
         <v>54</v>
       </c>
@@ -25083,8 +26268,14 @@
       <c r="G7" s="10">
         <v>1.6</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L7" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="M7" s="16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D8" s="1" t="s">
         <v>56</v>
       </c>
@@ -25097,8 +26288,14 @@
       <c r="G8" s="10">
         <v>1.65</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L8" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="M8" s="16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D9" s="1" t="s">
         <v>57</v>
       </c>
@@ -25111,8 +26308,14 @@
       <c r="G9" s="10">
         <v>1.75</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L9" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="M9" s="16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D10" s="1" t="s">
         <v>58</v>
       </c>
@@ -25125,8 +26328,14 @@
       <c r="G10" s="10">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L10" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="M10" s="16" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D11" s="1" t="s">
         <v>60</v>
       </c>
@@ -25139,8 +26348,14 @@
       <c r="G11" s="10">
         <v>1.75</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L11" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="M11" s="16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D12" s="1" t="s">
         <v>62</v>
       </c>
@@ -25154,7 +26369,7 @@
         <v>1.95</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D13" s="1" t="s">
         <v>64</v>
       </c>
@@ -25168,7 +26383,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D14" s="1" t="s">
         <v>65</v>
       </c>
@@ -25182,7 +26397,7 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D15" s="1" t="s">
         <v>66</v>
       </c>
@@ -25196,7 +26411,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D16" s="1" t="s">
         <v>68</v>
       </c>
@@ -26203,6 +27418,7 @@
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <phoneticPr fontId="9" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="G18" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
   </hyperlinks>

</xml_diff>

<commit_message>
add variable names to all four dataset
</commit_message>
<xml_diff>
--- a/Fichiers analyse/FOSSE 1-4.xlsx
+++ b/Fichiers analyse/FOSSE 1-4.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a648334db5f9744c/M2_EFT_projet_pedologie/Fichiers analyse/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cleme\Documents\GitHub\savoirs\cours\M2-pédologie\M2_EFT_projet_pedologie\Fichiers analyse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="80" documentId="13_ncr:1_{1523FAB1-26F5-4D24-B03C-72B0E9F713AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5986954-CBBC-4BE1-93D8-375E1E063016}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E94277DE-04B5-49DD-8EB1-C469994A1564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fosse1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1651" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1666" uniqueCount="93">
   <si>
     <t>Face</t>
   </si>
@@ -410,7 +410,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -438,7 +438,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -657,18 +656,18 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J1000"/>
+  <dimension ref="A1:O1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="K1" sqref="K1:O1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="6" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>22</v>
       </c>
@@ -699,8 +698,23 @@
       <c r="J1" s="13" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K1" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="L1" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="M1" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="N1" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="O1" s="15" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -733,7 +747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -766,7 +780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -799,7 +813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -832,7 +846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -865,7 +879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -898,7 +912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -931,7 +945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -964,7 +978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -997,7 +1011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -1030,7 +1044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -1063,7 +1077,7 @@
         <v>1.35</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1096,7 +1110,7 @@
         <v>1.35</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -1129,7 +1143,7 @@
         <v>1.35</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
@@ -1162,7 +1176,7 @@
         <v>1.35</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
@@ -4912,11 +4926,11 @@
   </sheetPr>
   <dimension ref="A1:O1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="O52" sqref="O52"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:O1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.6640625" customWidth="1"/>
     <col min="2" max="2" width="11.44140625" customWidth="1"/>
@@ -6361,7 +6375,7 @@
       <c r="N32" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="O32" s="17">
+      <c r="O32">
         <v>5</v>
       </c>
     </row>
@@ -6406,7 +6420,7 @@
       <c r="N33" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="O33" s="17">
+      <c r="O33">
         <v>5</v>
       </c>
     </row>
@@ -6451,7 +6465,7 @@
       <c r="N34" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="O34" s="17">
+      <c r="O34">
         <v>5</v>
       </c>
     </row>
@@ -6496,7 +6510,7 @@
       <c r="N35" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="O35" s="17">
+      <c r="O35">
         <v>5</v>
       </c>
     </row>
@@ -6541,7 +6555,7 @@
       <c r="N36" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="O36" s="17">
+      <c r="O36">
         <v>5</v>
       </c>
     </row>
@@ -6586,7 +6600,7 @@
       <c r="N37" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="O37" s="17">
+      <c r="O37">
         <v>5</v>
       </c>
     </row>
@@ -6631,7 +6645,7 @@
       <c r="N38" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="O38" s="17">
+      <c r="O38">
         <v>5</v>
       </c>
     </row>
@@ -6676,7 +6690,7 @@
       <c r="N39" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="O39" s="17">
+      <c r="O39">
         <v>5</v>
       </c>
     </row>
@@ -6721,7 +6735,7 @@
       <c r="N40" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="O40" s="17">
+      <c r="O40">
         <v>5</v>
       </c>
     </row>
@@ -6766,7 +6780,7 @@
       <c r="N41" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="O41" s="17">
+      <c r="O41">
         <v>5</v>
       </c>
     </row>
@@ -6811,7 +6825,7 @@
       <c r="N42" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="O42" s="17">
+      <c r="O42">
         <v>7.5</v>
       </c>
     </row>
@@ -6856,7 +6870,7 @@
       <c r="N43" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="O43" s="17">
+      <c r="O43">
         <v>7.5</v>
       </c>
     </row>
@@ -6901,7 +6915,7 @@
       <c r="N44" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="O44" s="17">
+      <c r="O44">
         <v>7.5</v>
       </c>
     </row>
@@ -6946,7 +6960,7 @@
       <c r="N45" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="O45" s="17">
+      <c r="O45">
         <v>7.5</v>
       </c>
     </row>
@@ -6991,7 +7005,7 @@
       <c r="N46" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="O46" s="17">
+      <c r="O46">
         <v>7.5</v>
       </c>
     </row>
@@ -7036,7 +7050,7 @@
       <c r="N47" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="O47" s="17">
+      <c r="O47">
         <v>7.5</v>
       </c>
     </row>
@@ -7081,7 +7095,7 @@
       <c r="N48" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="O48" s="17">
+      <c r="O48">
         <v>7.5</v>
       </c>
     </row>
@@ -7126,7 +7140,7 @@
       <c r="N49" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="O49" s="17">
+      <c r="O49">
         <v>7.5</v>
       </c>
     </row>
@@ -7171,7 +7185,7 @@
       <c r="N50" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="O50" s="17">
+      <c r="O50">
         <v>7.5</v>
       </c>
     </row>
@@ -7216,7 +7230,7 @@
       <c r="N51" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="O51" s="17">
+      <c r="O51">
         <v>7.5</v>
       </c>
     </row>
@@ -10232,11 +10246,11 @@
   </sheetPr>
   <dimension ref="A1:AA1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="G53" sqref="G53"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:O1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="6" width="12.6640625" customWidth="1"/>
   </cols>
@@ -10272,11 +10286,21 @@
       <c r="J1" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
+      <c r="K1" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="L1" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="M1" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="N1" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="O1" s="15" t="s">
+        <v>92</v>
+      </c>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
@@ -21800,18 +21824,18 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J1000"/>
+  <dimension ref="A1:O1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="G72" sqref="G72"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="6" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>22</v>
       </c>
@@ -21842,8 +21866,23 @@
       <c r="J1" s="13" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K1" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="L1" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="M1" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="N1" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="O1" s="15" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -21876,7 +21915,7 @@
         <v>1.35</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -21909,7 +21948,7 @@
         <v>1.35</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -21942,7 +21981,7 @@
         <v>1.35</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -21975,7 +22014,7 @@
         <v>1.35</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -22008,7 +22047,7 @@
         <v>1.35</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -22041,7 +22080,7 @@
         <v>1.35</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -22074,7 +22113,7 @@
         <v>1.35</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -22107,7 +22146,7 @@
         <v>1.35</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -22140,7 +22179,7 @@
         <v>1.35</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -22173,7 +22212,7 @@
         <v>1.35</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -22206,7 +22245,7 @@
         <v>1.35</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -22239,7 +22278,7 @@
         <v>1.35</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -22272,7 +22311,7 @@
         <v>1.35</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
@@ -22305,7 +22344,7 @@
         <v>1.35</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
@@ -26059,7 +26098,7 @@
       <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="6" width="12.6640625" customWidth="1"/>
   </cols>

</xml_diff>